<commit_message>
After some investigation into the required memory necesary for the whole system, I determined that the required memory would exceed 128MB available on the Nexys 4 board.  Therefore the Zedboard would need to be used since it contains 512MB of memory.  I also realized my current design was fundamentally flawed and a redesign would be needed.  After a few days of pencil and paper redesign, I implemented the new structure and am finishing the code currently.
</commit_message>
<xml_diff>
--- a/Xilinx_Projects/Thesis_CNN/Convolution_Parameters.xlsx
+++ b/Xilinx_Projects/Thesis_CNN/Convolution_Parameters.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4188"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,11 +477,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,10 +556,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D3" s="1">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -712,14 +712,14 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
       </c>
       <c r="C11" s="1">
         <f>((D3-D7)/B11)+1</f>
-        <v>55</v>
+        <v>54.25</v>
       </c>
       <c r="D11" s="1"/>
       <c r="I11" s="1">
@@ -794,11 +794,11 @@
       </c>
       <c r="B15" s="1">
         <f>1 + ((C3 + 2 * A11 - C7)/B11)</f>
-        <v>56</v>
+        <v>56.75</v>
       </c>
       <c r="C15" s="1">
         <f>1 + ((D3 + 2 * A11 - D7)/B11)</f>
-        <v>56</v>
+        <v>56.75</v>
       </c>
       <c r="D15" s="1"/>
       <c r="I15" s="1">

</xml_diff>